<commit_message>
see description - various changes
various bug fixes; deleted CROSP pond outputs; removed climate scaling; fixed units issue; refined and tested single calibration data inputs; adjusted notebook markdown to reflect changes; moved repo filepath to main code block; updated input files to Eagle pond per approval from parks;
</commit_message>
<xml_diff>
--- a/inputs/elev_calib_empty.xlsx
+++ b/inputs/elev_calib_empty.xlsx
@@ -2,18 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\218136\python_repo\Pond-IT\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E8C4CB-1AA6-4020-8936-E4C3628C03DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23ADD15-BE05-4D11-B928-796FA506AB4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="26610" windowHeight="16440" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="25" r:id="rId1"/>
+    <sheet name="Eagle" sheetId="25" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -396,6 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F93746C-0038-480A-954D-9FA4BDD9391F}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>